<commit_message>
work slowly go on
</commit_message>
<xml_diff>
--- a/Graf/Stany_wersja_4.xlsx
+++ b/Graf/Stany_wersja_4.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krzysiek\Documents\PROGRAMMING\REPOSITORY\AP_swiatla\Graf\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="45">
   <si>
     <t>A1</t>
   </si>
@@ -159,7 +154,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -238,7 +233,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="72">
+  <borders count="76">
     <border>
       <left/>
       <right/>
@@ -1179,11 +1174,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1397,33 +1438,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1443,12 +1457,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1477,33 +1485,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1521,6 +1508,82 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1583,7 +1646,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1618,7 +1681,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1795,7 +1858,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1803,10 +1866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL1000"/>
+  <dimension ref="A1:AP1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AN13" sqref="AN13"/>
+      <selection activeCell="B22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1817,77 +1880,77 @@
     <col min="38" max="38" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C2" s="88" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="88" t="s">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="C2" s="109" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="110"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="109" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="110"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="89"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="88" t="s">
+      <c r="J2" s="110"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="89"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="88" t="s">
+      <c r="M2" s="110"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="88" t="s">
+      <c r="P2" s="110"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="109" t="s">
         <v>5</v>
       </c>
-      <c r="S2" s="89"/>
-      <c r="T2" s="90"/>
-      <c r="U2" s="88" t="s">
+      <c r="S2" s="110"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="109" t="s">
         <v>6</v>
       </c>
-      <c r="V2" s="89"/>
-      <c r="W2" s="90"/>
-      <c r="X2" s="88" t="s">
+      <c r="V2" s="110"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="Y2" s="89"/>
-      <c r="Z2" s="90"/>
-      <c r="AA2" s="88" t="s">
+      <c r="Y2" s="110"/>
+      <c r="Z2" s="111"/>
+      <c r="AA2" s="109" t="s">
         <v>8</v>
       </c>
-      <c r="AB2" s="89"/>
-      <c r="AC2" s="90"/>
-      <c r="AD2" s="88" t="s">
+      <c r="AB2" s="110"/>
+      <c r="AC2" s="111"/>
+      <c r="AD2" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="AE2" s="89"/>
-      <c r="AF2" s="89"/>
-      <c r="AG2" s="88" t="s">
+      <c r="AE2" s="110"/>
+      <c r="AF2" s="110"/>
+      <c r="AG2" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="AH2" s="91"/>
-      <c r="AI2" s="88" t="s">
+      <c r="AH2" s="112"/>
+      <c r="AI2" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="AJ2" s="91"/>
+      <c r="AJ2" s="112"/>
       <c r="AK2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AL2" s="110" t="s">
+      <c r="AL2" s="95" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1993,8 +2056,8 @@
       <c r="AK3" s="7"/>
       <c r="AL3" s="49"/>
     </row>
-    <row r="4" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="s">
+    <row r="4" spans="1:42" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="122" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -2106,9 +2169,18 @@
         <v>15</v>
       </c>
       <c r="AL4" s="49"/>
-    </row>
-    <row r="5" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="100"/>
+      <c r="AN4" s="130" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP4" s="129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="123"/>
       <c r="B5" s="15" t="s">
         <v>16</v>
       </c>
@@ -2218,9 +2290,18 @@
         <v>17</v>
       </c>
       <c r="AL5" s="49"/>
-    </row>
-    <row r="6" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="100"/>
+      <c r="AN5" s="131" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP5" s="129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="123"/>
       <c r="B6" s="15" t="s">
         <v>18</v>
       </c>
@@ -2330,10 +2411,19 @@
         <v>20</v>
       </c>
       <c r="AL6" s="49"/>
-    </row>
-    <row r="7" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="100"/>
-      <c r="B7" s="92" t="s">
+      <c r="AN6" s="130" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP6" s="129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="123"/>
+      <c r="B7" s="79" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="54">
@@ -2441,513 +2531,567 @@
       <c r="AK7" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="AL7" s="110" t="s">
+      <c r="AL7" s="95" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A8" s="100"/>
-      <c r="B8" s="101" t="s">
+      <c r="AN7" s="131" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO7" s="79" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP7" s="129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="123"/>
+      <c r="B8" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="102">
-        <v>0</v>
-      </c>
-      <c r="D8" s="103">
-        <v>0</v>
-      </c>
-      <c r="E8" s="104">
-        <v>1</v>
-      </c>
-      <c r="F8" s="105">
-        <v>0</v>
-      </c>
-      <c r="G8" s="103">
-        <v>1</v>
-      </c>
-      <c r="H8" s="104">
-        <v>0</v>
-      </c>
-      <c r="I8" s="102">
-        <v>0</v>
-      </c>
-      <c r="J8" s="103">
-        <v>0</v>
-      </c>
-      <c r="K8" s="104">
-        <v>1</v>
-      </c>
-      <c r="L8" s="102">
-        <v>0</v>
-      </c>
-      <c r="M8" s="103">
-        <v>0</v>
-      </c>
-      <c r="N8" s="104">
-        <v>1</v>
-      </c>
-      <c r="O8" s="102">
-        <v>0</v>
-      </c>
-      <c r="P8" s="103">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="104">
-        <v>0</v>
-      </c>
-      <c r="R8" s="102">
-        <v>0</v>
-      </c>
-      <c r="S8" s="103">
-        <v>0</v>
-      </c>
-      <c r="T8" s="104">
-        <v>1</v>
-      </c>
-      <c r="U8" s="102">
-        <v>0</v>
-      </c>
-      <c r="V8" s="103">
-        <v>0</v>
-      </c>
-      <c r="W8" s="104">
-        <v>1</v>
-      </c>
-      <c r="X8" s="102">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="103">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="104">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="102">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="103">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="104">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="102">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="103">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="106">
-        <v>1</v>
-      </c>
-      <c r="AG8" s="102">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="106">
-        <v>1</v>
-      </c>
-      <c r="AI8" s="102">
-        <v>0</v>
-      </c>
-      <c r="AJ8" s="104">
-        <v>1</v>
-      </c>
-      <c r="AK8" s="107" t="s">
+      <c r="C8" s="87">
+        <v>0</v>
+      </c>
+      <c r="D8" s="88">
+        <v>0</v>
+      </c>
+      <c r="E8" s="89">
+        <v>1</v>
+      </c>
+      <c r="F8" s="90">
+        <v>0</v>
+      </c>
+      <c r="G8" s="88">
+        <v>1</v>
+      </c>
+      <c r="H8" s="89">
+        <v>0</v>
+      </c>
+      <c r="I8" s="87">
+        <v>0</v>
+      </c>
+      <c r="J8" s="88">
+        <v>0</v>
+      </c>
+      <c r="K8" s="89">
+        <v>1</v>
+      </c>
+      <c r="L8" s="87">
+        <v>0</v>
+      </c>
+      <c r="M8" s="88">
+        <v>0</v>
+      </c>
+      <c r="N8" s="89">
+        <v>1</v>
+      </c>
+      <c r="O8" s="87">
+        <v>0</v>
+      </c>
+      <c r="P8" s="88">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="89">
+        <v>0</v>
+      </c>
+      <c r="R8" s="87">
+        <v>0</v>
+      </c>
+      <c r="S8" s="88">
+        <v>0</v>
+      </c>
+      <c r="T8" s="89">
+        <v>1</v>
+      </c>
+      <c r="U8" s="87">
+        <v>0</v>
+      </c>
+      <c r="V8" s="88">
+        <v>0</v>
+      </c>
+      <c r="W8" s="89">
+        <v>1</v>
+      </c>
+      <c r="X8" s="87">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="88">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="89">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="87">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="88">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="89">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="87">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="88">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="91">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="87">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="91">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="87">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="89">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="92" t="s">
         <v>23</v>
       </c>
       <c r="AL8" s="49"/>
-    </row>
-    <row r="9" spans="1:38" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="112"/>
-      <c r="B9" s="108" t="s">
+      <c r="AN8" s="130" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO8" s="86" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP8" s="129">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="124"/>
+      <c r="B9" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="102">
-        <v>0</v>
-      </c>
-      <c r="D9" s="103">
-        <v>0</v>
-      </c>
-      <c r="E9" s="104">
-        <v>1</v>
-      </c>
-      <c r="F9" s="105">
-        <v>0</v>
-      </c>
-      <c r="G9" s="103">
-        <v>0</v>
-      </c>
-      <c r="H9" s="104">
-        <v>1</v>
-      </c>
-      <c r="I9" s="102">
-        <v>0</v>
-      </c>
-      <c r="J9" s="103">
-        <v>0</v>
-      </c>
-      <c r="K9" s="104">
-        <v>1</v>
-      </c>
-      <c r="L9" s="102">
-        <v>0</v>
-      </c>
-      <c r="M9" s="103">
-        <v>0</v>
-      </c>
-      <c r="N9" s="104">
-        <v>1</v>
-      </c>
-      <c r="O9" s="102">
-        <v>0</v>
-      </c>
-      <c r="P9" s="103">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="104">
-        <v>1</v>
-      </c>
-      <c r="R9" s="102">
-        <v>0</v>
-      </c>
-      <c r="S9" s="103">
-        <v>0</v>
-      </c>
-      <c r="T9" s="104">
-        <v>1</v>
-      </c>
-      <c r="U9" s="102">
-        <v>0</v>
-      </c>
-      <c r="V9" s="103">
-        <v>0</v>
-      </c>
-      <c r="W9" s="104">
-        <v>1</v>
-      </c>
-      <c r="X9" s="102">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="103">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="104">
-        <v>1</v>
-      </c>
-      <c r="AA9" s="102">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="103">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="104">
-        <v>1</v>
-      </c>
-      <c r="AD9" s="102">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="103">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="106">
-        <v>1</v>
-      </c>
-      <c r="AG9" s="102">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="106">
-        <v>1</v>
-      </c>
-      <c r="AI9" s="102">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="104">
-        <v>1</v>
-      </c>
-      <c r="AK9" s="109" t="s">
+      <c r="C9" s="87">
+        <v>0</v>
+      </c>
+      <c r="D9" s="88">
+        <v>0</v>
+      </c>
+      <c r="E9" s="89">
+        <v>1</v>
+      </c>
+      <c r="F9" s="90">
+        <v>0</v>
+      </c>
+      <c r="G9" s="88">
+        <v>0</v>
+      </c>
+      <c r="H9" s="89">
+        <v>1</v>
+      </c>
+      <c r="I9" s="87">
+        <v>0</v>
+      </c>
+      <c r="J9" s="88">
+        <v>0</v>
+      </c>
+      <c r="K9" s="89">
+        <v>1</v>
+      </c>
+      <c r="L9" s="87">
+        <v>0</v>
+      </c>
+      <c r="M9" s="88">
+        <v>0</v>
+      </c>
+      <c r="N9" s="89">
+        <v>1</v>
+      </c>
+      <c r="O9" s="87">
+        <v>0</v>
+      </c>
+      <c r="P9" s="88">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="89">
+        <v>1</v>
+      </c>
+      <c r="R9" s="87">
+        <v>0</v>
+      </c>
+      <c r="S9" s="88">
+        <v>0</v>
+      </c>
+      <c r="T9" s="89">
+        <v>1</v>
+      </c>
+      <c r="U9" s="87">
+        <v>0</v>
+      </c>
+      <c r="V9" s="88">
+        <v>0</v>
+      </c>
+      <c r="W9" s="89">
+        <v>1</v>
+      </c>
+      <c r="X9" s="87">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="88">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="89">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="87">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="88">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="89">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="87">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="88">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="91">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="87">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="91">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="87">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="89">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="AL9" s="110" t="s">
+      <c r="AL9" s="95" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:38" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="113" t="s">
+      <c r="AN9" s="131" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO9" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP9" s="129">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="120" t="s">
+      <c r="B10" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="121" t="s">
+      <c r="C10" s="128" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="122"/>
-      <c r="E10" s="122"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="122"/>
-      <c r="H10" s="122"/>
-      <c r="I10" s="122"/>
-      <c r="J10" s="122"/>
-      <c r="K10" s="122"/>
-      <c r="L10" s="122"/>
-      <c r="M10" s="122"/>
-      <c r="N10" s="122"/>
-      <c r="O10" s="122"/>
-      <c r="P10" s="122"/>
-      <c r="Q10" s="122"/>
-      <c r="R10" s="122"/>
-      <c r="S10" s="122"/>
-      <c r="T10" s="122"/>
-      <c r="U10" s="122"/>
-      <c r="V10" s="122"/>
-      <c r="W10" s="122"/>
-      <c r="X10" s="122"/>
-      <c r="Y10" s="122"/>
-      <c r="Z10" s="122"/>
-      <c r="AA10" s="122"/>
-      <c r="AB10" s="122"/>
-      <c r="AC10" s="122"/>
-      <c r="AD10" s="122"/>
-      <c r="AE10" s="122"/>
-      <c r="AF10" s="122"/>
-      <c r="AG10" s="122"/>
-      <c r="AH10" s="122"/>
-      <c r="AI10" s="122"/>
-      <c r="AJ10" s="122"/>
-      <c r="AK10" s="123"/>
-      <c r="AL10" s="110" t="s">
+      <c r="D10" s="138"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="138"/>
+      <c r="H10" s="138"/>
+      <c r="I10" s="138"/>
+      <c r="J10" s="138"/>
+      <c r="K10" s="138"/>
+      <c r="L10" s="138"/>
+      <c r="M10" s="138"/>
+      <c r="N10" s="138"/>
+      <c r="O10" s="138"/>
+      <c r="P10" s="138"/>
+      <c r="Q10" s="138"/>
+      <c r="R10" s="138"/>
+      <c r="S10" s="138"/>
+      <c r="T10" s="138"/>
+      <c r="U10" s="138"/>
+      <c r="V10" s="138"/>
+      <c r="W10" s="138"/>
+      <c r="X10" s="138"/>
+      <c r="Y10" s="138"/>
+      <c r="Z10" s="138"/>
+      <c r="AA10" s="138"/>
+      <c r="AB10" s="138"/>
+      <c r="AC10" s="138"/>
+      <c r="AD10" s="138"/>
+      <c r="AE10" s="138"/>
+      <c r="AF10" s="138"/>
+      <c r="AG10" s="138"/>
+      <c r="AH10" s="138"/>
+      <c r="AI10" s="138"/>
+      <c r="AJ10" s="138"/>
+      <c r="AK10" s="137"/>
+      <c r="AL10" s="95" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A11" s="114"/>
-      <c r="B11" s="124" t="s">
+      <c r="AN10" s="132" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO10" s="101" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP10" s="129">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="126"/>
+      <c r="B11" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="125">
-        <v>0</v>
-      </c>
-      <c r="D11" s="126">
-        <v>1</v>
-      </c>
-      <c r="E11" s="127">
-        <v>1</v>
-      </c>
-      <c r="F11" s="128">
-        <v>0</v>
-      </c>
-      <c r="G11" s="126">
-        <v>1</v>
-      </c>
-      <c r="H11" s="127">
-        <v>1</v>
-      </c>
-      <c r="I11" s="128">
-        <v>0</v>
-      </c>
-      <c r="J11" s="126">
-        <v>0</v>
-      </c>
-      <c r="K11" s="127">
-        <v>1</v>
-      </c>
-      <c r="L11" s="128">
-        <v>0</v>
-      </c>
-      <c r="M11" s="126">
-        <v>1</v>
-      </c>
-      <c r="N11" s="127">
-        <v>1</v>
-      </c>
-      <c r="O11" s="128">
-        <v>0</v>
-      </c>
-      <c r="P11" s="126">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="127">
-        <v>1</v>
-      </c>
-      <c r="R11" s="128">
-        <v>0</v>
-      </c>
-      <c r="S11" s="126">
-        <v>0</v>
-      </c>
-      <c r="T11" s="127">
-        <v>1</v>
-      </c>
-      <c r="U11" s="128">
-        <v>0</v>
-      </c>
-      <c r="V11" s="126">
-        <v>0</v>
-      </c>
-      <c r="W11" s="127">
-        <v>1</v>
-      </c>
-      <c r="X11" s="128">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="126">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="127">
-        <v>1</v>
-      </c>
-      <c r="AA11" s="128">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="126">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="127">
-        <v>1</v>
-      </c>
-      <c r="AD11" s="128">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="126">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="129">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="128">
-        <v>0</v>
-      </c>
-      <c r="AH11" s="129">
-        <v>1</v>
-      </c>
-      <c r="AI11" s="128">
-        <v>0</v>
-      </c>
-      <c r="AJ11" s="129">
-        <v>1</v>
-      </c>
-      <c r="AK11" s="130" t="s">
+      <c r="C11" s="103">
+        <v>0</v>
+      </c>
+      <c r="D11" s="104">
+        <v>1</v>
+      </c>
+      <c r="E11" s="105">
+        <v>1</v>
+      </c>
+      <c r="F11" s="106">
+        <v>0</v>
+      </c>
+      <c r="G11" s="104">
+        <v>1</v>
+      </c>
+      <c r="H11" s="105">
+        <v>1</v>
+      </c>
+      <c r="I11" s="106">
+        <v>0</v>
+      </c>
+      <c r="J11" s="104">
+        <v>0</v>
+      </c>
+      <c r="K11" s="105">
+        <v>1</v>
+      </c>
+      <c r="L11" s="106">
+        <v>0</v>
+      </c>
+      <c r="M11" s="104">
+        <v>1</v>
+      </c>
+      <c r="N11" s="105">
+        <v>1</v>
+      </c>
+      <c r="O11" s="106">
+        <v>0</v>
+      </c>
+      <c r="P11" s="104">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="105">
+        <v>1</v>
+      </c>
+      <c r="R11" s="106">
+        <v>0</v>
+      </c>
+      <c r="S11" s="104">
+        <v>0</v>
+      </c>
+      <c r="T11" s="105">
+        <v>1</v>
+      </c>
+      <c r="U11" s="106">
+        <v>0</v>
+      </c>
+      <c r="V11" s="104">
+        <v>0</v>
+      </c>
+      <c r="W11" s="105">
+        <v>1</v>
+      </c>
+      <c r="X11" s="106">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="104">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="105">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="106">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="104">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="105">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="106">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="104">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="107">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="106">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="107">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="106">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="107">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="AL11" s="110" t="s">
+      <c r="AL11" s="95" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="114"/>
-      <c r="B12" s="117" t="s">
+      <c r="AN11" s="132" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO11" s="102" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP11" s="129">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="126"/>
+      <c r="B12" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="93">
-        <v>0</v>
-      </c>
-      <c r="D12" s="94">
-        <v>1</v>
-      </c>
-      <c r="E12" s="95">
-        <v>1</v>
-      </c>
-      <c r="F12" s="96">
-        <v>1</v>
-      </c>
-      <c r="G12" s="94">
-        <v>0</v>
-      </c>
-      <c r="H12" s="95">
-        <v>0</v>
-      </c>
-      <c r="I12" s="96">
-        <v>0</v>
-      </c>
-      <c r="J12" s="94">
-        <v>0</v>
-      </c>
-      <c r="K12" s="95">
-        <v>1</v>
-      </c>
-      <c r="L12" s="96">
-        <v>0</v>
-      </c>
-      <c r="M12" s="94">
-        <v>1</v>
-      </c>
-      <c r="N12" s="95">
-        <v>1</v>
-      </c>
-      <c r="O12" s="96">
-        <v>1</v>
-      </c>
-      <c r="P12" s="94">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="95">
-        <v>0</v>
-      </c>
-      <c r="R12" s="96">
-        <v>0</v>
-      </c>
-      <c r="S12" s="94">
-        <v>0</v>
-      </c>
-      <c r="T12" s="95">
-        <v>1</v>
-      </c>
-      <c r="U12" s="96">
-        <v>0</v>
-      </c>
-      <c r="V12" s="94">
-        <v>0</v>
-      </c>
-      <c r="W12" s="95">
-        <v>1</v>
-      </c>
-      <c r="X12" s="96">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="94">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="95">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="96">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="94">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="95">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="96">
-        <v>0</v>
-      </c>
-      <c r="AE12" s="94">
-        <v>0</v>
-      </c>
-      <c r="AF12" s="97">
-        <v>1</v>
-      </c>
-      <c r="AG12" s="96">
-        <v>0</v>
-      </c>
-      <c r="AH12" s="97">
-        <v>1</v>
-      </c>
-      <c r="AI12" s="96">
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="97">
-        <v>1</v>
-      </c>
-      <c r="AK12" s="98" t="s">
+      <c r="C12" s="80">
+        <v>0</v>
+      </c>
+      <c r="D12" s="81">
+        <v>1</v>
+      </c>
+      <c r="E12" s="82">
+        <v>1</v>
+      </c>
+      <c r="F12" s="83">
+        <v>1</v>
+      </c>
+      <c r="G12" s="81">
+        <v>0</v>
+      </c>
+      <c r="H12" s="82">
+        <v>0</v>
+      </c>
+      <c r="I12" s="83">
+        <v>0</v>
+      </c>
+      <c r="J12" s="81">
+        <v>0</v>
+      </c>
+      <c r="K12" s="82">
+        <v>1</v>
+      </c>
+      <c r="L12" s="83">
+        <v>0</v>
+      </c>
+      <c r="M12" s="81">
+        <v>1</v>
+      </c>
+      <c r="N12" s="82">
+        <v>1</v>
+      </c>
+      <c r="O12" s="83">
+        <v>1</v>
+      </c>
+      <c r="P12" s="81">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="82">
+        <v>0</v>
+      </c>
+      <c r="R12" s="83">
+        <v>0</v>
+      </c>
+      <c r="S12" s="81">
+        <v>0</v>
+      </c>
+      <c r="T12" s="82">
+        <v>1</v>
+      </c>
+      <c r="U12" s="83">
+        <v>0</v>
+      </c>
+      <c r="V12" s="81">
+        <v>0</v>
+      </c>
+      <c r="W12" s="82">
+        <v>1</v>
+      </c>
+      <c r="X12" s="83">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="81">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="82">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="83">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="81">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="82">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="83">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="81">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="84">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="83">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="84">
+        <v>1</v>
+      </c>
+      <c r="AI12" s="83">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="84">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="85" t="s">
         <v>15</v>
       </c>
       <c r="AL12" s="49"/>
-    </row>
-    <row r="13" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="114"/>
-      <c r="B13" s="118" t="s">
+      <c r="AN12" s="132" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO12" s="98" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP12" s="129">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="126"/>
+      <c r="B13" s="99" t="s">
         <v>21</v>
       </c>
       <c r="C13" s="31">
@@ -3056,10 +3200,19 @@
         <v>17</v>
       </c>
       <c r="AL13" s="49"/>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A14" s="114"/>
-      <c r="B14" s="119" t="s">
+      <c r="AN13" s="132" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO13" s="99" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP13" s="129">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="126"/>
+      <c r="B14" s="100" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="31">
@@ -3168,10 +3321,19 @@
         <v>23</v>
       </c>
       <c r="AL14" s="49"/>
-    </row>
-    <row r="15" spans="1:38" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="115"/>
-      <c r="B15" s="116" t="s">
+      <c r="AN14" s="132" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO14" s="100" t="s">
+        <v>32</v>
+      </c>
+      <c r="AP14" s="129">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="127"/>
+      <c r="B15" s="97" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="37">
@@ -3279,12 +3441,21 @@
       <c r="AK15" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="AL15" s="110" t="s">
+      <c r="AL15" s="95" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:38" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="85" t="s">
+      <c r="AN15" s="132" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO15" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP15" s="129">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="118" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="42" t="s">
@@ -3396,9 +3567,18 @@
         <v>15</v>
       </c>
       <c r="AL16" s="49"/>
-    </row>
-    <row r="17" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
+      <c r="AN16" s="133" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO16" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP16" s="129">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="114"/>
       <c r="B17" s="43" t="s">
         <v>16</v>
       </c>
@@ -3508,9 +3688,18 @@
         <v>17</v>
       </c>
       <c r="AL17" s="49"/>
-    </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
+      <c r="AN17" s="133" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO17" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP17" s="129">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="114"/>
       <c r="B18" s="43" t="s">
         <v>18</v>
       </c>
@@ -3620,9 +3809,18 @@
         <v>23</v>
       </c>
       <c r="AL18" s="49"/>
-    </row>
-    <row r="19" spans="1:38" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="80"/>
+      <c r="AN18" s="133" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO18" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP18" s="129">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="114"/>
       <c r="B19" s="50" t="s">
         <v>21</v>
       </c>
@@ -3728,15 +3926,24 @@
       <c r="AJ19" s="55">
         <v>1</v>
       </c>
-      <c r="AK19" s="111" t="s">
+      <c r="AK19" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="AL19" s="110" t="s">
+      <c r="AL19" s="95" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:38" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="86" t="s">
+      <c r="AN19" s="133" t="s">
+        <v>24</v>
+      </c>
+      <c r="AO19" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP19" s="129">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="120" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="57" t="s">
@@ -3848,9 +4055,18 @@
         <v>15</v>
       </c>
       <c r="AL20" s="49"/>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A21" s="87"/>
+      <c r="AN20" s="134" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO20" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP20" s="129">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="121"/>
       <c r="B21" s="43" t="s">
         <v>16</v>
       </c>
@@ -3960,9 +4176,18 @@
         <v>26</v>
       </c>
       <c r="AL21" s="49"/>
-    </row>
-    <row r="22" spans="1:38" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="87"/>
+      <c r="AN21" s="134" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO21" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP21" s="129">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="121"/>
       <c r="B22" s="43" t="s">
         <v>18</v>
       </c>
@@ -4072,9 +4297,18 @@
         <v>20</v>
       </c>
       <c r="AL22" s="49"/>
-    </row>
-    <row r="23" spans="1:38" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="87"/>
+      <c r="AN22" s="134" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO22" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP22" s="129">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="121"/>
       <c r="B23" s="50" t="s">
         <v>21</v>
       </c>
@@ -4183,12 +4417,21 @@
       <c r="AK23" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="AL23" s="110" t="s">
+      <c r="AL23" s="95" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="84" t="s">
+      <c r="AN23" s="134" t="s">
+        <v>25</v>
+      </c>
+      <c r="AO23" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP23" s="129">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="119" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="75" t="s">
@@ -4300,9 +4543,18 @@
         <v>15</v>
       </c>
       <c r="AL24" s="49"/>
-    </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A25" s="80"/>
+      <c r="AN24" s="135" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO24" s="75" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP24" s="129">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="114"/>
       <c r="B25" s="76" t="s">
         <v>16</v>
       </c>
@@ -4412,9 +4664,18 @@
         <v>17</v>
       </c>
       <c r="AL25" s="49"/>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A26" s="80"/>
+      <c r="AN25" s="135" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO25" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP25" s="129">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="114"/>
       <c r="B26" s="76" t="s">
         <v>18</v>
       </c>
@@ -4524,9 +4785,18 @@
         <v>23</v>
       </c>
       <c r="AL26" s="49"/>
-    </row>
-    <row r="27" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="81"/>
+      <c r="AN26" s="135" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO26" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP26" s="129">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="115"/>
       <c r="B27" s="77" t="s">
         <v>21</v>
       </c>
@@ -4635,12 +4905,21 @@
       <c r="AK27" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="AL27" s="110" t="s">
+      <c r="AL27" s="95" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="79" t="s">
+      <c r="AN27" s="135" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO27" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP27" s="129">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="113" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="75" t="s">
@@ -4752,9 +5031,18 @@
         <v>15</v>
       </c>
       <c r="AL28" s="49"/>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A29" s="80"/>
+      <c r="AN28" s="136" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO28" s="75" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP28" s="129">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="114"/>
       <c r="B29" s="76" t="s">
         <v>16</v>
       </c>
@@ -4864,9 +5152,18 @@
         <v>17</v>
       </c>
       <c r="AL29" s="49"/>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A30" s="80"/>
+      <c r="AN29" s="136" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO29" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP29" s="129">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="114"/>
       <c r="B30" s="76" t="s">
         <v>18</v>
       </c>
@@ -4976,9 +5273,18 @@
         <v>23</v>
       </c>
       <c r="AL30" s="49"/>
-    </row>
-    <row r="31" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="81"/>
+      <c r="AN30" s="136" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO30" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="AP30" s="129">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="115"/>
       <c r="B31" s="77" t="s">
         <v>21</v>
       </c>
@@ -5087,11 +5393,20 @@
       <c r="AK31" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="AL31" s="110" t="s">
+      <c r="AL31" s="95" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:38" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AN31" s="136" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO31" s="77" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP31" s="129">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="O32" s="48"/>
       <c r="P32" s="48"/>
       <c r="Q32" s="48"/>
@@ -5110,38 +5425,38 @@
       <c r="AK34" s="1"/>
     </row>
     <row r="35" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I35" s="82" t="s">
+      <c r="I35" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="J35" s="83"/>
-      <c r="K35" s="83"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="83"/>
-      <c r="N35" s="83"/>
+      <c r="J35" s="117"/>
+      <c r="K35" s="117"/>
+      <c r="L35" s="117"/>
+      <c r="M35" s="117"/>
+      <c r="N35" s="117"/>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
     </row>
     <row r="36" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I36" s="82" t="s">
+      <c r="I36" s="116" t="s">
         <v>30</v>
       </c>
-      <c r="J36" s="83"/>
-      <c r="K36" s="83"/>
-      <c r="L36" s="83"/>
-      <c r="M36" s="83"/>
-      <c r="N36" s="83"/>
+      <c r="J36" s="117"/>
+      <c r="K36" s="117"/>
+      <c r="L36" s="117"/>
+      <c r="M36" s="117"/>
+      <c r="N36" s="117"/>
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
     </row>
     <row r="37" spans="9:37" x14ac:dyDescent="0.25">
-      <c r="I37" s="82" t="s">
+      <c r="I37" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="J37" s="83"/>
-      <c r="K37" s="83"/>
-      <c r="L37" s="83"/>
-      <c r="M37" s="83"/>
-      <c r="N37" s="83"/>
+      <c r="J37" s="117"/>
+      <c r="K37" s="117"/>
+      <c r="L37" s="117"/>
+      <c r="M37" s="117"/>
+      <c r="N37" s="117"/>
       <c r="O37" s="48"/>
       <c r="P37" s="48"/>
       <c r="Q37" s="48"/>
@@ -9002,6 +9317,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C10:AJ10"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="I35:N35"/>
+    <mergeCell ref="I36:N36"/>
+    <mergeCell ref="I37:N37"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A20:A23"/>
     <mergeCell ref="U2:W2"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="AG2:AH2"/>
@@ -9014,16 +9339,6 @@
     <mergeCell ref="AA2:AC2"/>
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="I35:N35"/>
-    <mergeCell ref="I36:N36"/>
-    <mergeCell ref="I37:N37"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="C10:AK10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>